<commit_message>
Contenu des messages passés en avro
</commit_message>
<xml_diff>
--- a/Gouvernance.xlsx
+++ b/Gouvernance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\git\kafka-demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EDBE8F-74EA-48D7-9B4F-2705F4769C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626830B1-F776-4701-8975-E4920A344AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18C22479-39DE-488C-B9F6-E2BD7DB1C7BF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Nom</t>
   </si>
@@ -106,6 +106,21 @@
   </si>
   <si>
     <t>Le topic a été supprimé des serveurs de production</t>
+  </si>
+  <si>
+    <t>Type clé</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Nb partitions</t>
+  </si>
+  <si>
+    <t>Schéma2</t>
+  </si>
+  <si>
+    <t>monitoring.cpu_v01.avsc</t>
   </si>
 </sst>
 </file>
@@ -161,15 +176,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD7F477-C1DE-4001-850A-4844B46A91B2}" name="Tableau1" displayName="Tableau1" ref="A1:G2" totalsRowShown="0">
-  <autoFilter ref="A1:G2" xr:uid="{3DD7F477-C1DE-4001-850A-4844B46A91B2}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD7F477-C1DE-4001-850A-4844B46A91B2}" name="Tableau1" displayName="Tableau1" ref="A1:J2" totalsRowShown="0">
+  <autoFilter ref="A1:J2" xr:uid="{3DD7F477-C1DE-4001-850A-4844B46A91B2}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{7D0A05FD-D527-442E-8767-1617C34971D2}" name="Nom"/>
     <tableColumn id="2" xr3:uid="{0507D762-9CB7-47DA-BAC0-8FE5FDB7F77B}" name="Description"/>
     <tableColumn id="7" xr3:uid="{FB228FC2-A294-4575-B423-63DD756A05C0}" name="Statut"/>
+    <tableColumn id="8" xr3:uid="{680B7C15-5500-4E59-A735-E5C265EE7397}" name="Type clé"/>
     <tableColumn id="3" xr3:uid="{D8EC54B9-441B-4FEB-869B-59D864EE0B8F}" name="Type données"/>
+    <tableColumn id="10" xr3:uid="{F5777FAF-28C1-432D-9C98-473911A8F1E0}" name="Schéma"/>
+    <tableColumn id="9" xr3:uid="{CF6FADD6-736D-4A0B-BB07-3C54699CF82F}" name="Nb partitions"/>
     <tableColumn id="6" xr3:uid="{1E10A871-F006-48A0-9B8F-E28B39ABEFEC}" name="Stratégie de versionning"/>
-    <tableColumn id="4" xr3:uid="{02519F93-AE2E-4875-B493-D8F7C8849E7C}" name="Schéma"/>
+    <tableColumn id="4" xr3:uid="{02519F93-AE2E-4875-B493-D8F7C8849E7C}" name="Schéma2"/>
     <tableColumn id="5" xr3:uid="{E9D6714F-B466-4ADD-8954-FB09F2248932}" name="version"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -484,24 +502,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8283E5-58DF-476E-A3CE-D77E9552B82A}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,19 +533,28 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -535,15 +565,24 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>1</v>
       </c>
     </row>

</xml_diff>